<commit_message>
Changing the value of 'Z' in the dataportal tests to 1.01 (following Dave's recent change to one of the examples).
</commit_message>
<xml_diff>
--- a/examples/pyomo/tutorials/excel.xlsx
+++ b/examples/pyomo/tutorials/excel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="100" windowWidth="19500" windowHeight="17960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2:AZ5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -696,7 +696,7 @@
         <v>31</v>
       </c>
       <c r="S2" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>0</v>

</xml_diff>